<commit_message>
udpated - optimimised performance
</commit_message>
<xml_diff>
--- a/Sample/Sample_forPCoding.xlsx
+++ b/Sample/Sample_forPCoding.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="gov" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="subdist" sheetId="2" r:id="rId3"/>
     <sheet name="Community" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -10834,7 +10834,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -11091,6 +11091,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -11126,6 +11143,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -12441,7 +12475,7 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12725,7 +12759,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>17</v>
       </c>
@@ -12742,7 +12776,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>17</v>
       </c>
@@ -12759,7 +12793,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>17</v>
       </c>
@@ -12776,7 +12810,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>17</v>
       </c>
@@ -12793,7 +12827,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>17</v>
       </c>
@@ -12810,7 +12844,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>17</v>
       </c>

</xml_diff>